<commit_message>
Rebuild JSON from updated ZNC07 Financial Performance Data and remove all fallback data
</commit_message>
<xml_diff>
--- a/public/ZNC07 Financial Performance Data.xlsx
+++ b/public/ZNC07 Financial Performance Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/Library/Mobile Documents/com~apple~CloudDocs/Wilmington Expense Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-ZNC07/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7879B2EF-2D55-E049-B692-5799327A767D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{68C778D5-2A93-954C-B2A5-E1C5ED5496F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="1280" windowWidth="28500" windowHeight="18360" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
+    <workbookView xWindow="2920" yWindow="760" windowWidth="25800" windowHeight="18880" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -342,7 +342,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -356,6 +362,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -375,17 +387,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -720,15 +744,15 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="33" hidden="1" customWidth="1"/>
     <col min="5" max="6" width="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.1640625" bestFit="1" customWidth="1"/>
@@ -775,13 +799,13 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>1235165.53</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>1095429.51</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="5">
         <f>(F2-E2)/E2</f>
         <v>-0.11313141162545236</v>
       </c>
@@ -803,18 +827,18 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>1157638.6399999999</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>1087941.57</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="5">
         <f>(F3-E3)/E3</f>
         <v>-6.0206240178714003E-2</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" ref="H3:H12" si="0">G3</f>
+        <f t="shared" ref="H3:H11" si="0">G3</f>
         <v>-6.0206240178714003E-2</v>
       </c>
     </row>
@@ -831,14 +855,14 @@
       <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>7171</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>6741</v>
       </c>
-      <c r="G4">
-        <f t="shared" ref="G3:G12" si="1">(F4-E4)/E4</f>
+      <c r="G4" s="5">
+        <f t="shared" ref="G4:G12" si="1">(F4-E4)/E4</f>
         <v>-5.9963742853158558E-2</v>
       </c>
       <c r="H4" s="1">
@@ -859,19 +883,19 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="E5">
-        <v>198222</v>
-      </c>
-      <c r="F5">
-        <v>192148</v>
-      </c>
-      <c r="G5">
+      <c r="E5" s="6">
+        <v>50753.18</v>
+      </c>
+      <c r="F5" s="4">
+        <v>42709.43</v>
+      </c>
+      <c r="G5" s="5">
         <f t="shared" si="1"/>
-        <v>-3.0642411034093087E-2</v>
+        <v>-0.15848760609680024</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="0"/>
-        <v>-3.0642411034093087E-2</v>
+        <v>-0.15848760609680024</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -887,19 +911,19 @@
       <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="E6">
-        <v>401969</v>
-      </c>
-      <c r="F6">
-        <v>439572</v>
-      </c>
-      <c r="G6">
+      <c r="E6" s="2">
+        <v>710873.33</v>
+      </c>
+      <c r="F6" s="4">
+        <v>558095.31999999995</v>
+      </c>
+      <c r="G6" s="5">
         <f t="shared" si="1"/>
-        <v>9.3547014819550758E-2</v>
+        <v>-0.21491594008738521</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
-        <v>9.3547014819550758E-2</v>
+        <v>-0.21491594008738521</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -915,19 +939,19 @@
       <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="E7">
-        <v>62401</v>
-      </c>
-      <c r="F7">
-        <v>47594</v>
-      </c>
-      <c r="G7">
+      <c r="E7" s="2">
+        <v>14847.88</v>
+      </c>
+      <c r="F7" s="4">
+        <v>22777.14</v>
+      </c>
+      <c r="G7" s="5">
         <f t="shared" si="1"/>
-        <v>-0.23728786397653884</v>
+        <v>0.53403314143163871</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="0"/>
-        <v>-0.23728786397653884</v>
+        <v>0.53403314143163871</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -943,19 +967,19 @@
       <c r="D8" t="s">
         <v>27</v>
       </c>
-      <c r="E8">
-        <v>33533</v>
-      </c>
-      <c r="F8">
-        <v>48384</v>
-      </c>
-      <c r="G8">
+      <c r="E8" s="2">
+        <v>71738.149999999994</v>
+      </c>
+      <c r="F8" s="4">
+        <v>69619.009999999995</v>
+      </c>
+      <c r="G8" s="5">
         <f t="shared" si="1"/>
-        <v>0.44287716577699582</v>
+        <v>-2.9539930985117396E-2</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>0.44287716577699582</v>
+        <v>-2.9539930985117396E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -971,19 +995,19 @@
       <c r="D9" t="s">
         <v>22</v>
       </c>
-      <c r="E9">
-        <v>6</v>
-      </c>
-      <c r="F9">
-        <v>8</v>
-      </c>
-      <c r="G9">
+      <c r="E9" s="2">
+        <v>72790.880000000005</v>
+      </c>
+      <c r="F9" s="4">
+        <v>87455.3</v>
+      </c>
+      <c r="G9" s="5">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.20145957845268525</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.20145957845268525</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -999,19 +1023,21 @@
       <c r="D10" t="s">
         <v>22</v>
       </c>
-      <c r="E10">
-        <v>145</v>
-      </c>
-      <c r="F10">
-        <v>138</v>
-      </c>
-      <c r="G10">
+      <c r="E10" s="3">
+        <f>E2/E4</f>
+        <v>172.24453074884954</v>
+      </c>
+      <c r="F10" s="3">
+        <f>F2/F4</f>
+        <v>162.502523364486</v>
+      </c>
+      <c r="G10" s="5">
         <f t="shared" si="1"/>
-        <v>-4.8275862068965517E-2</v>
+        <v>-5.6559168189603694E-2</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="0"/>
-        <v>-4.8275862068965517E-2</v>
+        <v>-5.6559168189603694E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1027,19 +1053,21 @@
       <c r="D11" t="s">
         <v>16</v>
       </c>
-      <c r="E11">
-        <v>105</v>
-      </c>
-      <c r="F11">
-        <v>137</v>
-      </c>
-      <c r="G11">
+      <c r="E11" s="3">
+        <f>E3/E4</f>
+        <v>161.43336215311672</v>
+      </c>
+      <c r="F11" s="3">
+        <f>F3/F4</f>
+        <v>161.39171784601692</v>
+      </c>
+      <c r="G11" s="5">
         <f t="shared" si="1"/>
-        <v>0.30476190476190479</v>
+        <v>-2.57965928135118E-4</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="0"/>
-        <v>0.30476190476190479</v>
+        <v>-2.57965928135118E-4</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1055,19 +1083,21 @@
       <c r="D12" t="s">
         <v>11</v>
       </c>
-      <c r="E12">
-        <v>-40</v>
-      </c>
-      <c r="F12">
-        <v>-1</v>
-      </c>
-      <c r="G12">
+      <c r="E12" s="3">
+        <f>E11-E10</f>
+        <v>-10.811168595732823</v>
+      </c>
+      <c r="F12" s="3">
+        <f>F11-F10</f>
+        <v>-1.1108055184690784</v>
+      </c>
+      <c r="G12" s="5">
         <f t="shared" si="1"/>
-        <v>-0.97499999999999998</v>
+        <v>-0.8972538899349406</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="0"/>
-        <v>-0.97499999999999998</v>
+        <f>G12*-1</f>
+        <v>0.8972538899349406</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1083,9 +1113,10 @@
       <c r="D13" t="s">
         <v>38</v>
       </c>
-      <c r="E13">
-        <v>405</v>
-      </c>
+      <c r="E13" s="6">
+        <v>1160</v>
+      </c>
+      <c r="F13" s="6"/>
       <c r="G13" t="s">
         <v>39</v>
       </c>
@@ -1106,8 +1137,10 @@
       <c r="D14" t="s">
         <v>41</v>
       </c>
-      <c r="F14">
-        <v>459</v>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6">
+        <f>E13*($H$4+1)</f>
+        <v>1090.442058290336</v>
       </c>
       <c r="G14" t="s">
         <v>39</v>
@@ -1129,8 +1162,9 @@
       <c r="D15" t="s">
         <v>41</v>
       </c>
-      <c r="F15">
-        <v>122566</v>
+      <c r="F15" s="7">
+        <f>F14*$F$10</f>
+        <v>177199.58605494353</v>
       </c>
       <c r="G15" t="s">
         <v>39</v>
@@ -1152,8 +1186,9 @@
       <c r="D16" t="s">
         <v>41</v>
       </c>
-      <c r="F16">
-        <v>62883</v>
+      <c r="F16" s="7">
+        <f>F14*$F$11</f>
+        <v>175988.31699902384</v>
       </c>
       <c r="G16" t="s">
         <v>39</v>
@@ -1175,9 +1210,9 @@
       <c r="D17" t="s">
         <v>41</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="7">
         <f>F16-F15</f>
-        <v>-59683</v>
+        <v>-1211.2690559196926</v>
       </c>
       <c r="G17" t="s">
         <v>39</v>
@@ -1199,8 +1234,9 @@
       <c r="D18" t="s">
         <v>41</v>
       </c>
-      <c r="F18">
-        <v>-18443</v>
+      <c r="F18" s="7">
+        <f>F17+17776</f>
+        <v>16564.730944080307</v>
       </c>
       <c r="G18" t="s">
         <v>39</v>
@@ -1222,8 +1258,8 @@
       <c r="D19" t="s">
         <v>38</v>
       </c>
-      <c r="E19">
-        <v>808</v>
+      <c r="E19" s="6">
+        <v>1050</v>
       </c>
       <c r="G19" t="s">
         <v>39</v>
@@ -1245,8 +1281,9 @@
       <c r="D20" t="s">
         <v>41</v>
       </c>
-      <c r="F20">
-        <v>915</v>
+      <c r="F20" s="9">
+        <f>E19*($H$4+1)</f>
+        <v>987.03807000418351</v>
       </c>
       <c r="G20" t="s">
         <v>39</v>
@@ -1268,8 +1305,9 @@
       <c r="D21" t="s">
         <v>41</v>
       </c>
-      <c r="F21">
-        <v>126280</v>
+      <c r="F21" s="7">
+        <f>F20*$F$10</f>
+        <v>160396.17703249201</v>
       </c>
       <c r="G21" t="s">
         <v>39</v>
@@ -1291,8 +1329,9 @@
       <c r="D22" t="s">
         <v>41</v>
       </c>
-      <c r="F22">
-        <v>125355</v>
+      <c r="F22" s="7">
+        <f>F20*$F$11</f>
+        <v>159299.76969739227</v>
       </c>
       <c r="G22" t="s">
         <v>39</v>
@@ -1314,9 +1353,9 @@
       <c r="D23" t="s">
         <v>41</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="8">
         <f>F22-F21</f>
-        <v>-925</v>
+        <v>-1096.4073350997351</v>
       </c>
       <c r="G23" t="s">
         <v>39</v>
@@ -1338,8 +1377,9 @@
       <c r="D24" t="s">
         <v>41</v>
       </c>
-      <c r="F24">
-        <v>-19358</v>
+      <c r="F24" s="8">
+        <f>F18+F23</f>
+        <v>15468.323608980572</v>
       </c>
       <c r="G24" t="s">
         <v>39</v>
@@ -1361,8 +1401,8 @@
       <c r="D25" t="s">
         <v>38</v>
       </c>
-      <c r="E25">
-        <v>784</v>
+      <c r="E25" s="6">
+        <v>1219</v>
       </c>
       <c r="G25" t="s">
         <v>39</v>
@@ -1384,8 +1424,10 @@
       <c r="D26" t="s">
         <v>41</v>
       </c>
-      <c r="F26">
-        <v>888</v>
+      <c r="E26" s="6"/>
+      <c r="F26" s="9">
+        <f>E25*($H$4+1)</f>
+        <v>1145.9041974619997</v>
       </c>
       <c r="G26" t="s">
         <v>39</v>
@@ -1407,8 +1449,9 @@
       <c r="D27" t="s">
         <v>41</v>
       </c>
-      <c r="F27">
-        <v>122529</v>
+      <c r="F27" s="7">
+        <f>F26*$F$10</f>
+        <v>186212.32362153119</v>
       </c>
       <c r="G27" t="s">
         <v>39</v>
@@ -1430,8 +1473,9 @@
       <c r="D28" t="s">
         <v>41</v>
       </c>
-      <c r="F28">
-        <v>121642</v>
+      <c r="F28" s="7">
+        <f>F26*$F$11</f>
+        <v>184939.4469153535</v>
       </c>
       <c r="G28" t="s">
         <v>39</v>
@@ -1453,9 +1497,9 @@
       <c r="D29" t="s">
         <v>41</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="8">
         <f>F28-F27</f>
-        <v>-887</v>
+        <v>-1272.8767061776889</v>
       </c>
       <c r="G29" t="s">
         <v>39</v>
@@ -1477,8 +1521,10 @@
       <c r="D30" t="s">
         <v>41</v>
       </c>
-      <c r="F30">
-        <v>-20246</v>
+      <c r="E30" s="6"/>
+      <c r="F30" s="8">
+        <f>F24+F29</f>
+        <v>14195.446902802883</v>
       </c>
       <c r="G30" t="s">
         <v>39</v>
@@ -1500,8 +1546,8 @@
       <c r="D31" t="s">
         <v>38</v>
       </c>
-      <c r="E31">
-        <v>830</v>
+      <c r="E31" s="6">
+        <v>1026</v>
       </c>
       <c r="G31" t="s">
         <v>39</v>
@@ -1523,8 +1569,10 @@
       <c r="D32" t="s">
         <v>41</v>
       </c>
-      <c r="F32">
-        <v>940</v>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6">
+        <f>E31*($H$4+1)</f>
+        <v>964.47719983265938</v>
       </c>
       <c r="G32" t="s">
         <v>39</v>
@@ -1546,8 +1594,10 @@
       <c r="D33" t="s">
         <v>41</v>
       </c>
-      <c r="F33">
-        <v>129719</v>
+      <c r="E33" s="6"/>
+      <c r="F33" s="7">
+        <f>F32*$F$10</f>
+        <v>156729.97870032076</v>
       </c>
       <c r="G33" t="s">
         <v>39</v>
@@ -1569,8 +1619,10 @@
       <c r="D34" t="s">
         <v>41</v>
       </c>
-      <c r="F34">
-        <v>128779</v>
+      <c r="E34" s="6"/>
+      <c r="F34" s="7">
+        <f>F32*$F$11</f>
+        <v>155658.63210430904</v>
       </c>
       <c r="G34" t="s">
         <v>39</v>
@@ -1592,9 +1644,10 @@
       <c r="D35" t="s">
         <v>41</v>
       </c>
-      <c r="F35">
+      <c r="E35" s="6"/>
+      <c r="F35" s="8">
         <f>F34-F33</f>
-        <v>-940</v>
+        <v>-1071.3465960117173</v>
       </c>
       <c r="G35" t="s">
         <v>39</v>
@@ -1616,8 +1669,10 @@
       <c r="D36" t="s">
         <v>41</v>
       </c>
-      <c r="F36">
-        <v>-21186</v>
+      <c r="E36" s="6"/>
+      <c r="F36" s="8">
+        <f>F30+F35</f>
+        <v>13124.100306791166</v>
       </c>
       <c r="G36" t="s">
         <v>39</v>
@@ -1639,8 +1694,8 @@
       <c r="D37" t="s">
         <v>38</v>
       </c>
-      <c r="E37">
-        <v>754</v>
+      <c r="E37" s="6">
+        <v>1030</v>
       </c>
       <c r="G37" t="s">
         <v>39</v>
@@ -1662,8 +1717,10 @@
       <c r="D38" t="s">
         <v>41</v>
       </c>
-      <c r="F38">
-        <v>854</v>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6">
+        <f>E37*($H$4+1)</f>
+        <v>968.2373448612467</v>
       </c>
       <c r="G38" t="s">
         <v>39</v>
@@ -1685,8 +1742,10 @@
       <c r="D39" t="s">
         <v>41</v>
       </c>
-      <c r="F39">
-        <v>117852</v>
+      <c r="E39" s="6"/>
+      <c r="F39" s="7">
+        <f>F38*$F$10</f>
+        <v>157341.01175568262</v>
       </c>
       <c r="G39" t="s">
         <v>39</v>
@@ -1708,8 +1767,9 @@
       <c r="D40" t="s">
         <v>41</v>
       </c>
-      <c r="F40">
-        <v>116998</v>
+      <c r="F40" s="7">
+        <f>F38*$F$11</f>
+        <v>156265.48836982291</v>
       </c>
       <c r="G40" t="s">
         <v>39</v>
@@ -1731,9 +1791,9 @@
       <c r="D41" t="s">
         <v>41</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="7">
         <f>F40-F39</f>
-        <v>-854</v>
+        <v>-1075.5233858597057</v>
       </c>
       <c r="G41" t="s">
         <v>39</v>
@@ -1755,8 +1815,9 @@
       <c r="D42" t="s">
         <v>41</v>
       </c>
-      <c r="F42">
-        <v>-22040</v>
+      <c r="F42" s="7">
+        <f>F36+F41</f>
+        <v>12048.57692093146</v>
       </c>
       <c r="G42" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Update financial performance data from Excel source
- Converted ZNC07 Financial Performance Data.xlsx to JSON
- Updated financial-performance-data.json with latest data (47 rows, 8 columns)
- Data includes YOY Expense & Profitability Analysis and Cashflow Projections
- Key metrics: Total Expenses (-11.3%), Total Revenue (-6.0%), Visit Count (-6.0%), Profit per Visit (+89.7%)
</commit_message>
<xml_diff>
--- a/public/ZNC07 Financial Performance Data.xlsx
+++ b/public/ZNC07 Financial Performance Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-ZNC07/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68C778D5-2A93-954C-B2A5-E1C5ED5496F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2303DD75-2285-D54A-8FAE-6023DCAB2D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="760" windowWidth="25800" windowHeight="18880" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
+    <workbookView xWindow="1020" yWindow="3900" windowWidth="29220" windowHeight="18880" xr2:uid="{D14BF5B3-A1B2-8F41-B345-A936FB541A15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="112">
   <si>
     <t>Metric_ID</t>
   </si>
@@ -336,6 +336,42 @@
   </si>
   <si>
     <t>CASHFLOW_DECEMBER_CASH_POSITION</t>
+  </si>
+  <si>
+    <t>VISITS_TO_GOAL</t>
+  </si>
+  <si>
+    <t>Visits to Goal</t>
+  </si>
+  <si>
+    <t>VISIT_STATUS_AUGUST</t>
+  </si>
+  <si>
+    <t>August 2025 End of Month Visit Status</t>
+  </si>
+  <si>
+    <t>September 2025 End of Month Visit Status</t>
+  </si>
+  <si>
+    <t>VISIT_STATUS_SEPTEMBER</t>
+  </si>
+  <si>
+    <t>VISIT_STATUS_OCTOBER</t>
+  </si>
+  <si>
+    <t>October 2025 End of Month Visit Status</t>
+  </si>
+  <si>
+    <t>VISIT_STATUS_NOVEMBER</t>
+  </si>
+  <si>
+    <t>November 2025 End of Month Visit Status</t>
+  </si>
+  <si>
+    <t>VISIT_STATUS_DECEMBER</t>
+  </si>
+  <si>
+    <t>December 2025 End of Month Visit Status</t>
   </si>
 </sst>
 </file>
@@ -348,7 +384,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -368,6 +404,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -393,7 +435,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -404,6 +446,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -741,15 +784,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FBEFE19-61E6-F243-A9CA-2FBB70397F74}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.5" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="33" hidden="1" customWidth="1"/>
@@ -1102,46 +1145,43 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="6">
-        <v>1160</v>
-      </c>
-      <c r="F13" s="6"/>
-      <c r="G13" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" t="s">
-        <v>39</v>
+        <v>16</v>
+      </c>
+      <c r="E13" s="10">
+        <f>-((E3-E2)/E11)</f>
+        <v>480.24081866341379</v>
+      </c>
+      <c r="F13" s="10">
+        <f>-((F3-F2)/F11)</f>
+        <v>46.396061086258172</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
         <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6">
-        <f>E13*($H$4+1)</f>
-        <v>1090.442058290336</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1160</v>
+      </c>
+      <c r="F14" s="3"/>
       <c r="G14" t="s">
         <v>39</v>
       </c>
@@ -1151,10 +1191,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
         <v>37</v>
@@ -1162,9 +1202,10 @@
       <c r="D15" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="7">
-        <f>F14*$F$10</f>
-        <v>177199.58605494353</v>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3">
+        <f>E14*($H$4+1)</f>
+        <v>1090.442058290336</v>
       </c>
       <c r="G15" t="s">
         <v>39</v>
@@ -1175,10 +1216,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
         <v>37</v>
@@ -1187,8 +1228,8 @@
         <v>41</v>
       </c>
       <c r="F16" s="7">
-        <f>F14*$F$11</f>
-        <v>175988.31699902384</v>
+        <f>F15*$F$10</f>
+        <v>177199.58605494353</v>
       </c>
       <c r="G16" t="s">
         <v>39</v>
@@ -1199,10 +1240,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
         <v>37</v>
@@ -1211,8 +1252,8 @@
         <v>41</v>
       </c>
       <c r="F17" s="7">
-        <f>F16-F15</f>
-        <v>-1211.2690559196926</v>
+        <f>F15*$F$11</f>
+        <v>175988.31699902384</v>
       </c>
       <c r="G17" t="s">
         <v>39</v>
@@ -1223,10 +1264,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
         <v>37</v>
@@ -1235,8 +1276,8 @@
         <v>41</v>
       </c>
       <c r="F18" s="7">
-        <f>F17+17776</f>
-        <v>16564.730944080307</v>
+        <f>F17-F16</f>
+        <v>-1211.2690559196926</v>
       </c>
       <c r="G18" t="s">
         <v>39</v>
@@ -1247,19 +1288,20 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="C19" t="s">
         <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="6">
-        <v>1050</v>
+        <v>41</v>
+      </c>
+      <c r="F19" s="3">
+        <f>(F18/$F$11)</f>
+        <v>-7.5051500292930688</v>
       </c>
       <c r="G19" t="s">
         <v>39</v>
@@ -1270,10 +1312,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
         <v>37</v>
@@ -1281,9 +1323,9 @@
       <c r="D20" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="9">
-        <f>E19*($H$4+1)</f>
-        <v>987.03807000418351</v>
+      <c r="F20" s="7">
+        <f>F18+17776</f>
+        <v>16564.730944080307</v>
       </c>
       <c r="G20" t="s">
         <v>39</v>
@@ -1294,21 +1336,21 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
         <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="7">
-        <f>F20*$F$10</f>
-        <v>160396.17703249201</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1050</v>
+      </c>
+      <c r="F21" s="3"/>
       <c r="G21" t="s">
         <v>39</v>
       </c>
@@ -1318,10 +1360,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
         <v>37</v>
@@ -1329,9 +1371,10 @@
       <c r="D22" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="7">
-        <f>F20*$F$11</f>
-        <v>159299.76969739227</v>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3">
+        <f>E21*($H$4+1)</f>
+        <v>987.03807000418351</v>
       </c>
       <c r="G22" t="s">
         <v>39</v>
@@ -1342,10 +1385,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
         <v>37</v>
@@ -1353,9 +1396,9 @@
       <c r="D23" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="8">
-        <f>F22-F21</f>
-        <v>-1096.4073350997351</v>
+      <c r="F23" s="7">
+        <f>F22*$F$10</f>
+        <v>160396.17703249201</v>
       </c>
       <c r="G23" t="s">
         <v>39</v>
@@ -1366,10 +1409,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C24" t="s">
         <v>37</v>
@@ -1377,9 +1420,9 @@
       <c r="D24" t="s">
         <v>41</v>
       </c>
-      <c r="F24" s="8">
-        <f>F18+F23</f>
-        <v>15468.323608980572</v>
+      <c r="F24" s="7">
+        <f>F22*$F$11</f>
+        <v>159299.76969739227</v>
       </c>
       <c r="G24" t="s">
         <v>39</v>
@@ -1390,19 +1433,20 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s">
         <v>37</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
-      </c>
-      <c r="E25" s="6">
-        <v>1219</v>
+        <v>41</v>
+      </c>
+      <c r="F25" s="8">
+        <f>F24-F23</f>
+        <v>-1096.4073350997351</v>
       </c>
       <c r="G25" t="s">
         <v>39</v>
@@ -1413,10 +1457,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>104</v>
       </c>
       <c r="C26" t="s">
         <v>37</v>
@@ -1424,10 +1468,9 @@
       <c r="D26" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="9">
-        <f>E25*($H$4+1)</f>
-        <v>1145.9041974619997</v>
+      <c r="F26" s="3">
+        <f>(F25/$F$11)</f>
+        <v>-6.7934547678946711</v>
       </c>
       <c r="G26" t="s">
         <v>39</v>
@@ -1438,10 +1481,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
         <v>37</v>
@@ -1449,9 +1492,9 @@
       <c r="D27" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="7">
-        <f>F26*$F$10</f>
-        <v>186212.32362153119</v>
+      <c r="F27" s="8">
+        <f>F20+F25</f>
+        <v>15468.323608980572</v>
       </c>
       <c r="G27" t="s">
         <v>39</v>
@@ -1462,20 +1505,19 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C28" t="s">
         <v>37</v>
       </c>
       <c r="D28" t="s">
-        <v>41</v>
-      </c>
-      <c r="F28" s="7">
-        <f>F26*$F$11</f>
-        <v>184939.4469153535</v>
+        <v>38</v>
+      </c>
+      <c r="E28" s="6">
+        <v>1219</v>
       </c>
       <c r="G28" t="s">
         <v>39</v>
@@ -1486,10 +1528,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
         <v>37</v>
@@ -1497,9 +1539,10 @@
       <c r="D29" t="s">
         <v>41</v>
       </c>
-      <c r="F29" s="8">
-        <f>F28-F27</f>
-        <v>-1272.8767061776889</v>
+      <c r="E29" s="6"/>
+      <c r="F29" s="9">
+        <f>E28*($H$4+1)</f>
+        <v>1145.9041974619997</v>
       </c>
       <c r="G29" t="s">
         <v>39</v>
@@ -1510,10 +1553,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C30" t="s">
         <v>37</v>
@@ -1521,10 +1564,9 @@
       <c r="D30" t="s">
         <v>41</v>
       </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="8">
-        <f>F24+F29</f>
-        <v>14195.446902802883</v>
+      <c r="F30" s="7">
+        <f>F29*$F$10</f>
+        <v>186212.32362153119</v>
       </c>
       <c r="G30" t="s">
         <v>39</v>
@@ -1535,19 +1577,20 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C31" t="s">
         <v>37</v>
       </c>
       <c r="D31" t="s">
-        <v>38</v>
-      </c>
-      <c r="E31" s="6">
-        <v>1026</v>
+        <v>41</v>
+      </c>
+      <c r="F31" s="7">
+        <f>F29*$F$11</f>
+        <v>184939.4469153535</v>
       </c>
       <c r="G31" t="s">
         <v>39</v>
@@ -1558,10 +1601,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C32" t="s">
         <v>37</v>
@@ -1569,10 +1612,9 @@
       <c r="D32" t="s">
         <v>41</v>
       </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6">
-        <f>E31*($H$4+1)</f>
-        <v>964.47719983265938</v>
+      <c r="F32" s="8">
+        <f>F31-F30</f>
+        <v>-1272.8767061776889</v>
       </c>
       <c r="G32" t="s">
         <v>39</v>
@@ -1583,10 +1625,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="C33" t="s">
         <v>37</v>
@@ -1594,10 +1636,9 @@
       <c r="D33" t="s">
         <v>41</v>
       </c>
-      <c r="E33" s="6"/>
-      <c r="F33" s="7">
-        <f>F32*$F$10</f>
-        <v>156729.97870032076</v>
+      <c r="F33" s="3">
+        <f>(F32/$F$11)</f>
+        <v>-7.8868774876796008</v>
       </c>
       <c r="G33" t="s">
         <v>39</v>
@@ -1608,10 +1649,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B34" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C34" t="s">
         <v>37</v>
@@ -1620,9 +1661,9 @@
         <v>41</v>
       </c>
       <c r="E34" s="6"/>
-      <c r="F34" s="7">
-        <f>F32*$F$11</f>
-        <v>155658.63210430904</v>
+      <c r="F34" s="8">
+        <f>F27+F32</f>
+        <v>14195.446902802883</v>
       </c>
       <c r="G34" t="s">
         <v>39</v>
@@ -1633,21 +1674,19 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B35" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s">
         <v>37</v>
       </c>
       <c r="D35" t="s">
-        <v>41</v>
-      </c>
-      <c r="E35" s="6"/>
-      <c r="F35" s="8">
-        <f>F34-F33</f>
-        <v>-1071.3465960117173</v>
+        <v>38</v>
+      </c>
+      <c r="E35" s="6">
+        <v>1026</v>
       </c>
       <c r="G35" t="s">
         <v>39</v>
@@ -1658,10 +1697,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C36" t="s">
         <v>37</v>
@@ -1670,9 +1709,9 @@
         <v>41</v>
       </c>
       <c r="E36" s="6"/>
-      <c r="F36" s="8">
-        <f>F30+F35</f>
-        <v>13124.100306791166</v>
+      <c r="F36" s="6">
+        <f>E35*($H$4+1)</f>
+        <v>964.47719983265938</v>
       </c>
       <c r="G36" t="s">
         <v>39</v>
@@ -1683,19 +1722,21 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B37" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C37" t="s">
         <v>37</v>
       </c>
       <c r="D37" t="s">
-        <v>38</v>
-      </c>
-      <c r="E37" s="6">
-        <v>1030</v>
+        <v>41</v>
+      </c>
+      <c r="E37" s="6"/>
+      <c r="F37" s="7">
+        <f>F36*$F$10</f>
+        <v>156729.97870032076</v>
       </c>
       <c r="G37" t="s">
         <v>39</v>
@@ -1706,10 +1747,10 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="C38" t="s">
         <v>37</v>
@@ -1718,9 +1759,9 @@
         <v>41</v>
       </c>
       <c r="E38" s="6"/>
-      <c r="F38" s="6">
-        <f>E37*($H$4+1)</f>
-        <v>968.2373448612467</v>
+      <c r="F38" s="7">
+        <f>F36*$F$11</f>
+        <v>155658.63210430904</v>
       </c>
       <c r="G38" t="s">
         <v>39</v>
@@ -1731,10 +1772,10 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B39" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C39" t="s">
         <v>37</v>
@@ -1743,9 +1784,9 @@
         <v>41</v>
       </c>
       <c r="E39" s="6"/>
-      <c r="F39" s="7">
-        <f>F38*$F$10</f>
-        <v>157341.01175568262</v>
+      <c r="F39" s="8">
+        <f>F38-F37</f>
+        <v>-1071.3465960117173</v>
       </c>
       <c r="G39" t="s">
         <v>39</v>
@@ -1756,10 +1797,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="C40" t="s">
         <v>37</v>
@@ -1767,9 +1808,9 @@
       <c r="D40" t="s">
         <v>41</v>
       </c>
-      <c r="F40" s="7">
-        <f>F38*$F$11</f>
-        <v>156265.48836982291</v>
+      <c r="F40" s="3">
+        <f>(F39/$F$11)</f>
+        <v>-6.6381758017712169</v>
       </c>
       <c r="G40" t="s">
         <v>39</v>
@@ -1780,10 +1821,10 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B41" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C41" t="s">
         <v>37</v>
@@ -1791,9 +1832,10 @@
       <c r="D41" t="s">
         <v>41</v>
       </c>
-      <c r="F41" s="7">
-        <f>F40-F39</f>
-        <v>-1075.5233858597057</v>
+      <c r="E41" s="6"/>
+      <c r="F41" s="8">
+        <f>F34+F39</f>
+        <v>13124.100306791166</v>
       </c>
       <c r="G41" t="s">
         <v>39</v>
@@ -1804,25 +1846,170 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" s="6">
+        <v>1030</v>
+      </c>
+      <c r="G42" t="s">
+        <v>39</v>
+      </c>
+      <c r="H42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" t="s">
+        <v>41</v>
+      </c>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6">
+        <f>E42*($H$4+1)</f>
+        <v>968.2373448612467</v>
+      </c>
+      <c r="G43" t="s">
+        <v>39</v>
+      </c>
+      <c r="H43" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" s="6"/>
+      <c r="F44" s="7">
+        <f>F43*$F$10</f>
+        <v>157341.01175568262</v>
+      </c>
+      <c r="G44" t="s">
+        <v>39</v>
+      </c>
+      <c r="H44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" t="s">
+        <v>41</v>
+      </c>
+      <c r="F45" s="7">
+        <f>F43*$F$11</f>
+        <v>156265.48836982291</v>
+      </c>
+      <c r="G45" t="s">
+        <v>39</v>
+      </c>
+      <c r="H45" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46" t="s">
+        <v>41</v>
+      </c>
+      <c r="F46" s="7">
+        <f>F45-F44</f>
+        <v>-1075.5233858597057</v>
+      </c>
+      <c r="G46" t="s">
+        <v>39</v>
+      </c>
+      <c r="H46" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>110</v>
+      </c>
+      <c r="B47" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47" t="s">
+        <v>37</v>
+      </c>
+      <c r="D47" t="s">
+        <v>41</v>
+      </c>
+      <c r="F47" s="3">
+        <f>(F46/$F$11)</f>
+        <v>-6.6640556294583693</v>
+      </c>
+      <c r="G47" t="s">
+        <v>39</v>
+      </c>
+      <c r="H47" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>99</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B48" t="s">
         <v>47</v>
       </c>
-      <c r="C42" t="s">
-        <v>37</v>
-      </c>
-      <c r="D42" t="s">
-        <v>41</v>
-      </c>
-      <c r="F42" s="7">
-        <f>F36+F41</f>
+      <c r="C48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" t="s">
+        <v>41</v>
+      </c>
+      <c r="F48" s="7">
+        <f>F41+F46</f>
         <v>12048.57692093146</v>
       </c>
-      <c r="G42" t="s">
-        <v>39</v>
-      </c>
-      <c r="H42" t="s">
+      <c r="G48" t="s">
+        <v>39</v>
+      </c>
+      <c r="H48" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>